<commit_message>
Estadisticos Segundo Parcial 26 Mayo
</commit_message>
<xml_diff>
--- a/DetalleXDocente20242.xlsx
+++ b/DetalleXDocente20242.xlsx
@@ -9318,22 +9318,22 @@
         <v>16</v>
       </c>
       <c r="F251">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G251" s="1">
         <v>69.59999999999999</v>
       </c>
       <c r="H251" s="1">
-        <v>26.1</v>
+        <v>30.4</v>
       </c>
       <c r="I251" s="2">
-        <v>7.9</v>
+        <v>7.8</v>
       </c>
       <c r="J251">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K251" s="1">
-        <v>4.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:11">
@@ -9385,22 +9385,22 @@
         <v>33</v>
       </c>
       <c r="F253">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G253" s="1">
         <v>82.5</v>
       </c>
       <c r="H253" s="1">
-        <v>15</v>
+        <v>17.5</v>
       </c>
       <c r="I253" s="2">
-        <v>8.699999999999999</v>
+        <v>8.6</v>
       </c>
       <c r="J253">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K253" s="1">
-        <v>2.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="254" spans="1:11">
@@ -11930,22 +11930,25 @@
         <v>28</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F8">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="G8" s="1">
-        <v>0</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="H8" s="1">
-        <v>100</v>
+        <v>21.4</v>
+      </c>
+      <c r="I8" s="2">
+        <v>7.5</v>
       </c>
       <c r="J8">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="K8" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -12099,25 +12102,25 @@
         <v>147</v>
       </c>
       <c r="E13">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="F13">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="G13" s="1">
-        <v>64.59999999999999</v>
+        <v>79.59999999999999</v>
       </c>
       <c r="H13" s="1">
-        <v>35.4</v>
+        <v>20.4</v>
       </c>
       <c r="I13" s="2">
         <v>7.4</v>
       </c>
       <c r="J13">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="K13" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -15921,22 +15924,25 @@
         <v>15</v>
       </c>
       <c r="E127">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F127">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G127" s="1">
-        <v>0</v>
+        <v>93.3</v>
       </c>
       <c r="H127" s="1">
-        <v>100</v>
+        <v>6.7</v>
+      </c>
+      <c r="I127" s="2">
+        <v>8.300000000000001</v>
       </c>
       <c r="J127">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="K127" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:11">
@@ -15953,22 +15959,25 @@
         <v>25</v>
       </c>
       <c r="E128">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F128">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="G128" s="1">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="H128" s="1">
-        <v>100</v>
+        <v>4</v>
+      </c>
+      <c r="I128" s="2">
+        <v>8.4</v>
       </c>
       <c r="J128">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="K128" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:11">
@@ -15982,22 +15991,25 @@
         <v>40</v>
       </c>
       <c r="E129">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="F129">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="G129" s="1">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="H129" s="1">
-        <v>100</v>
+        <v>5</v>
+      </c>
+      <c r="I129" s="2">
+        <v>8.4</v>
       </c>
       <c r="J129">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="K129" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:11">
@@ -17025,22 +17037,25 @@
         <v>35</v>
       </c>
       <c r="E160">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="F160">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="G160" s="1">
-        <v>0</v>
+        <v>97.09999999999999</v>
       </c>
       <c r="H160" s="1">
-        <v>100</v>
+        <v>2.9</v>
+      </c>
+      <c r="I160" s="2">
+        <v>6.9</v>
       </c>
       <c r="J160">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="K160" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:11">
@@ -17054,22 +17069,25 @@
         <v>35</v>
       </c>
       <c r="E161">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="F161">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="G161" s="1">
-        <v>0</v>
+        <v>97.09999999999999</v>
       </c>
       <c r="H161" s="1">
-        <v>100</v>
+        <v>2.9</v>
+      </c>
+      <c r="I161" s="2">
+        <v>6.9</v>
       </c>
       <c r="J161">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="K161" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:11">
@@ -17500,22 +17518,25 @@
         <v>24</v>
       </c>
       <c r="E174">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F174">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="G174" s="1">
-        <v>0</v>
+        <v>83.3</v>
       </c>
       <c r="H174" s="1">
-        <v>100</v>
+        <v>16.7</v>
+      </c>
+      <c r="I174" s="2">
+        <v>7.6</v>
       </c>
       <c r="J174">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K174" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:11">
@@ -17710,10 +17731,10 @@
         <v>9.1</v>
       </c>
       <c r="J180">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K180" s="1">
-        <v>2.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181" spans="1:11">
@@ -17727,25 +17748,25 @@
         <v>191</v>
       </c>
       <c r="E181">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="F181">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="G181" s="1">
-        <v>84.8</v>
+        <v>95.3</v>
       </c>
       <c r="H181" s="1">
-        <v>15.2</v>
+        <v>4.7</v>
       </c>
       <c r="I181" s="2">
-        <v>8.9</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="J181">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="K181" s="1">
-        <v>13.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182" spans="1:11">
@@ -20102,22 +20123,25 @@
         <v>23</v>
       </c>
       <c r="E251">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F251">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="G251" s="1">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="H251" s="1">
-        <v>95.7</v>
+        <v>13</v>
+      </c>
+      <c r="I251" s="2">
+        <v>8.300000000000001</v>
       </c>
       <c r="J251">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K251" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:11">
@@ -20166,25 +20190,25 @@
         <v>40</v>
       </c>
       <c r="E253">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F253">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="G253" s="1">
-        <v>42.5</v>
+        <v>92.5</v>
       </c>
       <c r="H253" s="1">
-        <v>55</v>
+        <v>7.5</v>
       </c>
       <c r="I253" s="2">
-        <v>9.1</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="J253">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K253" s="1">
-        <v>57.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="254" spans="1:11">
@@ -20361,22 +20385,25 @@
         <v>11</v>
       </c>
       <c r="E259">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F259">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G259" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H259" s="1">
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="I259" s="2">
+        <v>8.6</v>
       </c>
       <c r="J259">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="K259" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="260" spans="1:11">
@@ -20393,22 +20420,25 @@
         <v>17</v>
       </c>
       <c r="E260">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F260">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="G260" s="1">
-        <v>0</v>
+        <v>94.09999999999999</v>
       </c>
       <c r="H260" s="1">
-        <v>100</v>
+        <v>5.9</v>
+      </c>
+      <c r="I260" s="2">
+        <v>8.5</v>
       </c>
       <c r="J260">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="K260" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="261" spans="1:11">
@@ -20425,22 +20455,25 @@
         <v>25</v>
       </c>
       <c r="E261">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F261">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="G261" s="1">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="H261" s="1">
-        <v>100</v>
+        <v>4</v>
+      </c>
+      <c r="I261" s="2">
+        <v>9.4</v>
       </c>
       <c r="J261">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="K261" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="262" spans="1:11">
@@ -20454,22 +20487,25 @@
         <v>53</v>
       </c>
       <c r="E262">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="F262">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="G262" s="1">
-        <v>0</v>
+        <v>96.2</v>
       </c>
       <c r="H262" s="1">
-        <v>100</v>
+        <v>3.8</v>
+      </c>
+      <c r="I262" s="2">
+        <v>8.800000000000001</v>
       </c>
       <c r="J262">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="K262" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="263" spans="1:11">
@@ -20643,25 +20679,25 @@
         <v>39</v>
       </c>
       <c r="E268">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="F268">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G268" s="1">
-        <v>56.4</v>
+        <v>100</v>
       </c>
       <c r="H268" s="1">
-        <v>43.6</v>
+        <v>0</v>
       </c>
       <c r="I268" s="2">
-        <v>9.9</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="J268">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="K268" s="1">
-        <v>43.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="269" spans="1:11">
@@ -20675,25 +20711,25 @@
         <v>39</v>
       </c>
       <c r="E269">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="F269">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G269" s="1">
-        <v>56.4</v>
+        <v>100</v>
       </c>
       <c r="H269" s="1">
-        <v>43.6</v>
+        <v>0</v>
       </c>
       <c r="I269" s="2">
-        <v>9.9</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="J269">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="K269" s="1">
-        <v>43.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="270" spans="1:11">
@@ -21164,22 +21200,25 @@
         <v>24</v>
       </c>
       <c r="E284">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F284">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="G284" s="1">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="H284" s="1">
-        <v>100</v>
+        <v>25</v>
+      </c>
+      <c r="I284" s="2">
+        <v>7.8</v>
       </c>
       <c r="J284">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K284" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="285" spans="1:11">
@@ -21196,22 +21235,25 @@
         <v>34</v>
       </c>
       <c r="E285">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F285">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="G285" s="1">
-        <v>0</v>
+        <v>94.09999999999999</v>
       </c>
       <c r="H285" s="1">
-        <v>100</v>
+        <v>5.9</v>
+      </c>
+      <c r="I285" s="2">
+        <v>8.5</v>
       </c>
       <c r="J285">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="K285" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="286" spans="1:11">
@@ -21228,22 +21270,25 @@
         <v>31</v>
       </c>
       <c r="E286">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="F286">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="G286" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H286" s="1">
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="I286" s="2">
+        <v>9</v>
       </c>
       <c r="J286">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K286" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="287" spans="1:11">
@@ -21260,22 +21305,25 @@
         <v>40</v>
       </c>
       <c r="E287">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F287">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G287" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H287" s="1">
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="I287" s="2">
+        <v>9.300000000000001</v>
       </c>
       <c r="J287">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="K287" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="288" spans="1:11">
@@ -21292,22 +21340,25 @@
         <v>24</v>
       </c>
       <c r="E288">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F288">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="G288" s="1">
-        <v>0</v>
+        <v>79.2</v>
       </c>
       <c r="H288" s="1">
-        <v>100</v>
+        <v>20.8</v>
+      </c>
+      <c r="I288" s="2">
+        <v>7.6</v>
       </c>
       <c r="J288">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K288" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="289" spans="1:11">
@@ -21324,22 +21375,25 @@
         <v>38</v>
       </c>
       <c r="E289">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="F289">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="G289" s="1">
-        <v>0</v>
+        <v>92.09999999999999</v>
       </c>
       <c r="H289" s="1">
-        <v>100</v>
+        <v>7.9</v>
+      </c>
+      <c r="I289" s="2">
+        <v>8.9</v>
       </c>
       <c r="J289">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="K289" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="290" spans="1:11">
@@ -21353,22 +21407,25 @@
         <v>191</v>
       </c>
       <c r="E290">
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="F290">
-        <v>191</v>
+        <v>16</v>
       </c>
       <c r="G290" s="1">
-        <v>0</v>
+        <v>91.59999999999999</v>
       </c>
       <c r="H290" s="1">
-        <v>100</v>
+        <v>8.4</v>
+      </c>
+      <c r="I290" s="2">
+        <v>8.5</v>
       </c>
       <c r="J290">
-        <v>191</v>
+        <v>0</v>
       </c>
       <c r="K290" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="291" spans="1:11">
@@ -21857,22 +21914,25 @@
         <v>36</v>
       </c>
       <c r="E305">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F305">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="G305" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H305" s="1">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="I305" s="2">
+        <v>7</v>
       </c>
       <c r="J305">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="K305" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="306" spans="1:11">
@@ -21889,22 +21949,25 @@
         <v>28</v>
       </c>
       <c r="E306">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F306">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="G306" s="1">
-        <v>0</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="H306" s="1">
-        <v>100</v>
+        <v>28.6</v>
+      </c>
+      <c r="I306" s="2">
+        <v>7.3</v>
       </c>
       <c r="J306">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="K306" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="307" spans="1:11">
@@ -21921,22 +21984,25 @@
         <v>23</v>
       </c>
       <c r="E307">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F307">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G307" s="1">
-        <v>0</v>
+        <v>52.2</v>
       </c>
       <c r="H307" s="1">
-        <v>100</v>
+        <v>47.8</v>
+      </c>
+      <c r="I307" s="2">
+        <v>6.9</v>
       </c>
       <c r="J307">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="K307" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="308" spans="1:11">
@@ -21953,22 +22019,25 @@
         <v>30</v>
       </c>
       <c r="E308">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F308">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G308" s="1">
-        <v>0</v>
+        <v>66.7</v>
       </c>
       <c r="H308" s="1">
-        <v>100</v>
+        <v>33.3</v>
+      </c>
+      <c r="I308" s="2">
+        <v>7.2</v>
       </c>
       <c r="J308">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K308" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="309" spans="1:11">
@@ -21985,22 +22054,25 @@
         <v>11</v>
       </c>
       <c r="E309">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F309">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G309" s="1">
-        <v>0</v>
+        <v>63.6</v>
       </c>
       <c r="H309" s="1">
-        <v>100</v>
+        <v>36.4</v>
+      </c>
+      <c r="I309" s="2">
+        <v>6.5</v>
       </c>
       <c r="J309">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="K309" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="310" spans="1:11">
@@ -22014,22 +22086,25 @@
         <v>128</v>
       </c>
       <c r="E310">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="F310">
-        <v>128</v>
+        <v>51</v>
       </c>
       <c r="G310" s="1">
-        <v>0</v>
+        <v>60.2</v>
       </c>
       <c r="H310" s="1">
-        <v>100</v>
+        <v>39.8</v>
+      </c>
+      <c r="I310" s="2">
+        <v>7</v>
       </c>
       <c r="J310">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K310" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="311" spans="1:11">
@@ -22663,19 +22738,19 @@
         <v>28</v>
       </c>
       <c r="E8">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F8">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="G8" s="1">
-        <v>42.9</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="H8" s="1">
-        <v>57.1</v>
+        <v>21.4</v>
       </c>
       <c r="I8" s="2">
-        <v>5.7</v>
+        <v>6.8</v>
       </c>
       <c r="J8">
         <v>28</v>
@@ -22835,19 +22910,19 @@
         <v>147</v>
       </c>
       <c r="E13">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="F13">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G13" s="1">
-        <v>72.8</v>
+        <v>79.59999999999999</v>
       </c>
       <c r="H13" s="1">
-        <v>27.2</v>
+        <v>20.4</v>
       </c>
       <c r="I13" s="2">
-        <v>6.7</v>
+        <v>6.9</v>
       </c>
       <c r="J13">
         <v>147</v>
@@ -26675,7 +26750,7 @@
         <v>6.7</v>
       </c>
       <c r="I127" s="2">
-        <v>7.9</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="J127">
         <v>15</v>
@@ -26698,19 +26773,19 @@
         <v>25</v>
       </c>
       <c r="E128">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F128">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G128" s="1">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="H128" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I128" s="2">
-        <v>7.6</v>
+        <v>8.4</v>
       </c>
       <c r="J128">
         <v>25</v>
@@ -26730,19 +26805,19 @@
         <v>40</v>
       </c>
       <c r="E129">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F129">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G129" s="1">
-        <v>92.5</v>
+        <v>95</v>
       </c>
       <c r="H129" s="1">
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="I129" s="2">
-        <v>7.8</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="J129">
         <v>40</v>
@@ -27788,7 +27863,7 @@
         <v>2.9</v>
       </c>
       <c r="I160" s="2">
-        <v>7.4</v>
+        <v>7.3</v>
       </c>
       <c r="J160">
         <v>35</v>
@@ -27820,7 +27895,7 @@
         <v>2.9</v>
       </c>
       <c r="I161" s="2">
-        <v>7.4</v>
+        <v>7.3</v>
       </c>
       <c r="J161">
         <v>35</v>
@@ -30862,19 +30937,19 @@
         <v>23</v>
       </c>
       <c r="E251">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F251">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G251" s="1">
-        <v>69.59999999999999</v>
+        <v>87</v>
       </c>
       <c r="H251" s="1">
-        <v>26.1</v>
+        <v>13</v>
       </c>
       <c r="I251" s="2">
-        <v>7.9</v>
+        <v>8.1</v>
       </c>
       <c r="J251">
         <v>23</v>
@@ -30929,19 +31004,19 @@
         <v>40</v>
       </c>
       <c r="E253">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F253">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G253" s="1">
-        <v>82.5</v>
+        <v>92.5</v>
       </c>
       <c r="H253" s="1">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="I253" s="2">
-        <v>8.699999999999999</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="J253">
         <v>40</v>
@@ -31136,7 +31211,7 @@
         <v>0</v>
       </c>
       <c r="I259" s="2">
-        <v>8.1</v>
+        <v>8.6</v>
       </c>
       <c r="J259">
         <v>11</v>
@@ -31171,7 +31246,7 @@
         <v>5.9</v>
       </c>
       <c r="I260" s="2">
-        <v>7.4</v>
+        <v>8.1</v>
       </c>
       <c r="J260">
         <v>17</v>
@@ -31206,7 +31281,7 @@
         <v>4</v>
       </c>
       <c r="I261" s="2">
-        <v>7.1</v>
+        <v>8.5</v>
       </c>
       <c r="J261">
         <v>25</v>
@@ -31238,7 +31313,7 @@
         <v>3.8</v>
       </c>
       <c r="I262" s="2">
-        <v>7.5</v>
+        <v>8.4</v>
       </c>
       <c r="J262">
         <v>53</v>
@@ -31418,19 +31493,19 @@
         <v>39</v>
       </c>
       <c r="E268">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F268">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G268" s="1">
-        <v>94.90000000000001</v>
+        <v>100</v>
       </c>
       <c r="H268" s="1">
-        <v>5.1</v>
+        <v>0</v>
       </c>
       <c r="I268" s="2">
-        <v>9.1</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="J268">
         <v>39</v>
@@ -31450,19 +31525,19 @@
         <v>39</v>
       </c>
       <c r="E269">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F269">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G269" s="1">
-        <v>94.90000000000001</v>
+        <v>100</v>
       </c>
       <c r="H269" s="1">
-        <v>5.1</v>
+        <v>0</v>
       </c>
       <c r="I269" s="2">
-        <v>9.1</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="J269">
         <v>39</v>
@@ -31951,7 +32026,7 @@
         <v>25</v>
       </c>
       <c r="I284" s="2">
-        <v>6.8</v>
+        <v>7.3</v>
       </c>
       <c r="J284">
         <v>24</v>
@@ -31986,7 +32061,7 @@
         <v>5.9</v>
       </c>
       <c r="I285" s="2">
-        <v>7.9</v>
+        <v>8.4</v>
       </c>
       <c r="J285">
         <v>34</v>
@@ -32009,19 +32084,19 @@
         <v>31</v>
       </c>
       <c r="E286">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F286">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G286" s="1">
-        <v>96.8</v>
+        <v>100</v>
       </c>
       <c r="H286" s="1">
-        <v>3.2</v>
+        <v>0</v>
       </c>
       <c r="I286" s="2">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="J286">
         <v>31</v>
@@ -32056,7 +32131,7 @@
         <v>0</v>
       </c>
       <c r="I287" s="2">
-        <v>8.9</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="J287">
         <v>40</v>
@@ -32079,19 +32154,19 @@
         <v>24</v>
       </c>
       <c r="E288">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F288">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G288" s="1">
-        <v>83.3</v>
+        <v>79.2</v>
       </c>
       <c r="H288" s="1">
-        <v>16.7</v>
+        <v>20.8</v>
       </c>
       <c r="I288" s="2">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="J288">
         <v>24</v>
@@ -32114,19 +32189,19 @@
         <v>38</v>
       </c>
       <c r="E289">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F289">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G289" s="1">
-        <v>86.8</v>
+        <v>92.09999999999999</v>
       </c>
       <c r="H289" s="1">
-        <v>13.2</v>
+        <v>7.9</v>
       </c>
       <c r="I289" s="2">
-        <v>8.800000000000001</v>
+        <v>9</v>
       </c>
       <c r="J289">
         <v>38</v>
@@ -32146,19 +32221,19 @@
         <v>191</v>
       </c>
       <c r="E290">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F290">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G290" s="1">
-        <v>90.59999999999999</v>
+        <v>91.59999999999999</v>
       </c>
       <c r="H290" s="1">
-        <v>9.4</v>
+        <v>8.4</v>
       </c>
       <c r="I290" s="2">
-        <v>8</v>
+        <v>8.4</v>
       </c>
       <c r="J290">
         <v>191</v>
@@ -32653,19 +32728,19 @@
         <v>36</v>
       </c>
       <c r="E305">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F305">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G305" s="1">
-        <v>30.6</v>
+        <v>50</v>
       </c>
       <c r="H305" s="1">
-        <v>69.40000000000001</v>
+        <v>50</v>
       </c>
       <c r="I305" s="2">
-        <v>5.8</v>
+        <v>6.2</v>
       </c>
       <c r="J305">
         <v>36</v>
@@ -32688,19 +32763,19 @@
         <v>28</v>
       </c>
       <c r="E306">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F306">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G306" s="1">
-        <v>60.7</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="H306" s="1">
-        <v>39.3</v>
+        <v>28.6</v>
       </c>
       <c r="I306" s="2">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="J306">
         <v>28</v>
@@ -32723,19 +32798,19 @@
         <v>23</v>
       </c>
       <c r="E307">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F307">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G307" s="1">
-        <v>43.5</v>
+        <v>52.2</v>
       </c>
       <c r="H307" s="1">
-        <v>56.5</v>
+        <v>47.8</v>
       </c>
       <c r="I307" s="2">
-        <v>6.2</v>
+        <v>6.4</v>
       </c>
       <c r="J307">
         <v>23</v>
@@ -32758,19 +32833,19 @@
         <v>30</v>
       </c>
       <c r="E308">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F308">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G308" s="1">
-        <v>53.3</v>
+        <v>66.7</v>
       </c>
       <c r="H308" s="1">
-        <v>46.7</v>
+        <v>33.3</v>
       </c>
       <c r="I308" s="2">
-        <v>6.6</v>
+        <v>6.9</v>
       </c>
       <c r="J308">
         <v>30</v>
@@ -32805,7 +32880,7 @@
         <v>36.4</v>
       </c>
       <c r="I309" s="2">
-        <v>6.7</v>
+        <v>6.5</v>
       </c>
       <c r="J309">
         <v>11</v>
@@ -32825,19 +32900,19 @@
         <v>128</v>
       </c>
       <c r="E310">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F310">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="G310" s="1">
-        <v>47.7</v>
+        <v>60.2</v>
       </c>
       <c r="H310" s="1">
-        <v>52.3</v>
+        <v>39.8</v>
       </c>
       <c r="I310" s="2">
-        <v>6.4</v>
+        <v>6.6</v>
       </c>
       <c r="J310">
         <v>128</v>

</xml_diff>